<commit_message>
2023 July 09 02:32pm
</commit_message>
<xml_diff>
--- a/Models/Fed Models/Four Models/Graphs/Correlation Table.xlsx
+++ b/Models/Fed Models/Four Models/Graphs/Correlation Table.xlsx
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2007_2009</t>
+          <t>2006_2007</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.3048</v>
+        <v>0.1058</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2007_2009</t>
+          <t>2006_2007</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -477,13 +477,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.2899</v>
+        <v>0.0143</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2007_2009</t>
+          <t>2006_2007</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -492,13 +492,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.1437</v>
+        <v>0.1327</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2007_2009</t>
+          <t>2006_2007</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -507,13 +507,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.3116</v>
+        <v>-0.0263</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2007_2009</t>
+          <t>2006_2007</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -522,232 +522,232 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.3264</v>
+        <v>-0.2366</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2008_2009</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>rate</t>
+          <t>credit</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5772</v>
+        <v>-0.5286999999999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2008_2009</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>credit</t>
+          <t>market</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.4083</v>
+        <v>0.2252</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2008_2009</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>market</t>
+          <t>rate</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.865</v>
+        <v>-0.6975</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2008_2009</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>inflation</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.4966</v>
+        <v>-0.1311</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2008_2009</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>inflation</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.7827</v>
+        <v>-0.4211</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2020_2021</t>
+          <t>2010_2019</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>market</t>
+          <t>rate</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.7118</v>
+        <v>0.5772</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2020_2021</t>
+          <t>2010_2019</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>inflation</t>
+          <t>credit</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.176</v>
+        <v>-0.4083</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2020_2021</t>
+          <t>2010_2019</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>rate</t>
+          <t>market</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.1858</v>
+        <v>0.865</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2020_2021</t>
+          <t>2010_2019</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>credit</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-0.0794</v>
+        <v>0.4966</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2020_2021</t>
+          <t>2010_2019</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>inflation</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.2283</v>
+        <v>0.7827</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2022_2023</t>
+          <t>2020_2023</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>rate</t>
+          <t>market</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.4956</v>
+        <v>0.643</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2022_2023</t>
+          <t>2020_2023</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>market</t>
+          <t>inflation</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.5197000000000001</v>
+        <v>0.5832000000000001</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2022_2023</t>
+          <t>2020_2023</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>inflation</t>
+          <t>rate</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.0374</v>
+        <v>0.7486</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2022_2023</t>
+          <t>2020_2023</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>credit</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.6238</v>
+        <v>0.4103</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2022_2023</t>
+          <t>2020_2023</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>credit</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.6752</v>
+        <v>0.8001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>